<commit_message>
Adding solar projection calc
</commit_message>
<xml_diff>
--- a/bash2.xlsx
+++ b/bash2.xlsx
@@ -14,19 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
-  <si>
-    <t>Task</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t xml:space="preserve">efficiency = tight coupling 
 </t>
   </si>
   <si>
-    <t xml:space="preserve">resilience = loose coupling 
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">goal build up utilities to couple to geometry and material
 </t>
   </si>
@@ -168,22 +161,40 @@
   </si>
   <si>
     <t>simulation utility = energy calculation from loads</t>
+  </si>
+  <si>
+    <t>Energy Production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Goals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">redundancy = loose coupling 
+</t>
+  </si>
+  <si>
+    <t>utlity for surface subdivision matrix</t>
+  </si>
+  <si>
+    <t>utlity for surface wedgin matrix</t>
+  </si>
+  <si>
+    <t>utlity for geometry differential vector and adjacency matrix</t>
+  </si>
+  <si>
+    <t>utility for adjacency map of thermal zones</t>
+  </si>
+  <si>
+    <t>Differential Geometry</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -226,10 +237,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -525,343 +546,313 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="71" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="3" width="71" style="1" customWidth="1"/>
+    <col min="4" max="4" width="67.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="69" style="1" customWidth="1"/>
+    <col min="6" max="6" width="74.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:6" ht="32.25" customHeight="1">
+      <c r="B1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="27.75" customHeight="1">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1">
+      <c r="B3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="D10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="D12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="E13" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="E14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="E15" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="E16" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="1">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="1">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="1">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="1">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="1">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="1">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="1">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="1">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="1">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="1">
-        <v>31</v>
-      </c>
-      <c r="B33" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="1">
-        <v>32</v>
-      </c>
-      <c r="B34" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="1">
-        <v>33</v>
-      </c>
-      <c r="B35" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="1">
-        <v>34</v>
-      </c>
-      <c r="B36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="1">
-        <v>35</v>
-      </c>
-      <c r="B37" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="1">
-        <v>36</v>
-      </c>
-      <c r="B38" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="1">
-        <v>37</v>
-      </c>
-      <c r="B39" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="1">
-        <v>38</v>
-      </c>
-      <c r="B40" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="1">
-        <v>39</v>
-      </c>
-      <c r="B41" t="s">
-        <v>38</v>
-      </c>
+    <row r="18" spans="1:1">
+      <c r="A18" s="3"/>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="3"/>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="3"/>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="3"/>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="3"/>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="3"/>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="3"/>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="3"/>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="3"/>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="3"/>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="3"/>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="3"/>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="3"/>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="3"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="3"/>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="3"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="3"/>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="3"/>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="3"/>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="3"/>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="3"/>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>